<commit_message>
Create more robust test case
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NWU\3rd Year\Semester 2\CMPG 323\Project 4\CMPG-323-Project4-30449960\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F937F30-AC95-4B32-BEFB-82CA5FD0F33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE646BFD-026F-48CC-9BFD-BE751D78A467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2715" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1178,7 @@
         <v>58</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>59</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
@@ -1229,7 +1229,7 @@
         <v>61</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -1314,7 +1314,7 @@
         <v>66</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
@@ -1331,7 +1331,7 @@
         <v>67</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>68</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
@@ -1365,7 +1365,7 @@
         <v>69</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
@@ -1382,7 +1382,7 @@
         <v>70</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
@@ -1399,7 +1399,7 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
@@ -1416,7 +1416,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
@@ -1450,7 +1450,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
@@ -1467,7 +1467,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
@@ -1484,7 +1484,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>
@@ -1501,7 +1501,7 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
@@ -1518,7 +1518,7 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
@@ -1535,7 +1535,7 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>

</xml_diff>